<commit_message>
Updated product backlog / sprints
</commit_message>
<xml_diff>
--- a/02-Sprint_Tracking/Sprints.xlsx
+++ b/02-Sprint_Tracking/Sprints.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\richa\Desktop\COMP1004-Coursework\02-Sprint_Tracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AC0E2E4-E81B-4AB3-96AC-528B7407448F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{629AC415-417C-46A3-9A90-B386D0025426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21120" xr2:uid="{743FDD4B-2014-4ECF-9DD7-51E90CC264F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
   <si>
     <t>Due Date</t>
   </si>
@@ -105,6 +105,27 @@
   </si>
   <si>
     <t>Implent an "Ultrawide" layout, displaying all three sections in a single row using flexboxes. Create relevant wireframe diagrams.</t>
+  </si>
+  <si>
+    <t>Implement a prototype of the View Page JavaScript to take test JSON data and display as a table</t>
+  </si>
+  <si>
+    <t>"Prettify" the above table; CSS</t>
+  </si>
+  <si>
+    <t>Update view.js to read and parse data from the real JSON database</t>
+  </si>
+  <si>
+    <t>Implement the HTML form to add new items to a JSON database</t>
+  </si>
+  <si>
+    <t>Investigate SQL / PostgreSQL as a relational database as opposed to JSON; check this fits CW limits?</t>
+  </si>
+  <si>
+    <t>Create "Interim Video"</t>
+  </si>
+  <si>
+    <t>Documentation</t>
   </si>
 </sst>
 </file>
@@ -469,7 +490,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -730,72 +751,126 @@
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>45252</v>
+      </c>
       <c r="B12" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C12" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>45259</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2"/>
+      <c r="G12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>45252</v>
+      </c>
       <c r="B13" s="1">
         <v>2</v>
       </c>
       <c r="C13" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>45266</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
+      <c r="G13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>45259</v>
+      </c>
       <c r="B14" s="1">
         <v>2</v>
       </c>
       <c r="C14" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>45273</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
+      <c r="G14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>45259</v>
+      </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>45273</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2"/>
+      <c r="G15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>45273</v>
+      </c>
       <c r="B16" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>45308</v>
       </c>
       <c r="E16" s="2"/>
       <c r="F16" s="2"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>45273</v>
+      </c>
       <c r="B17" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
-        <v>14</v>
+        <v>45308</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2"/>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B18" s="1">
         <v>2</v>
       </c>
@@ -806,7 +881,7 @@
       <c r="E18" s="2"/>
       <c r="F18" s="2"/>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B19" s="1">
         <v>2</v>
       </c>
@@ -817,7 +892,7 @@
       <c r="E19" s="2"/>
       <c r="F19" s="2"/>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B20" s="1">
         <v>2</v>
       </c>
@@ -828,7 +903,7 @@
       <c r="E20" s="2"/>
       <c r="F20" s="2"/>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B21" s="1">
         <v>2</v>
       </c>
@@ -839,7 +914,7 @@
       <c r="E21" s="2"/>
       <c r="F21" s="2"/>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B22" s="1">
         <v>2</v>
       </c>
@@ -850,7 +925,7 @@
       <c r="E22" s="2"/>
       <c r="F22" s="2"/>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B23" s="1">
         <v>2</v>
       </c>
@@ -861,7 +936,7 @@
       <c r="E23" s="2"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B24" s="1">
         <v>2</v>
       </c>
@@ -872,7 +947,7 @@
       <c r="E24" s="2"/>
       <c r="F24" s="2"/>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B25" s="1">
         <v>2</v>
       </c>
@@ -883,7 +958,7 @@
       <c r="E25" s="2"/>
       <c r="F25" s="2"/>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B26" s="1">
         <v>2</v>
       </c>
@@ -894,7 +969,7 @@
       <c r="E26" s="2"/>
       <c r="F26" s="2"/>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B27" s="1">
         <v>2</v>
       </c>
@@ -905,7 +980,7 @@
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B28" s="1">
         <v>2</v>
       </c>
@@ -916,7 +991,7 @@
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C29" s="2"/>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>

</xml_diff>